<commit_message>
Created UI and Analytics
</commit_message>
<xml_diff>
--- a/attendance/December 2024/CSE101/attendance.xlsx
+++ b/attendance/December 2024/CSE101/attendance.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tue 03-12-24" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -26,7 +25,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,10 +47,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -62,7 +72,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -427,11 +437,16 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="14.5546875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="20.5546875" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="16.5546875" bestFit="1" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">

</xml_diff>